<commit_message>
feat: add v2.0 mfg files
</commit_message>
<xml_diff>
--- a/MFG/V1.3_20230605/SMT/STARRYSKY_XY_JLC.xlsx
+++ b/MFG/V1.3_20230605/SMT/STARRYSKY_XY_JLC.xlsx
@@ -1752,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A559" workbookViewId="0">
-      <selection activeCell="A560" sqref="A560"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>